<commit_message>
Update portfolio.xlsx on 2025-08-17 07:21:44
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,36 @@
         <v>664.5999755859375</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>231.5899963378906</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>520.1699829101562</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>203.8999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>